<commit_message>
Added Link to Video
</commit_message>
<xml_diff>
--- a/GroupByWithDynamicDrillDown.xlsx
+++ b/GroupByWithDynamicDrillDown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10000001_{D654140C-F73A-4D3E-9AD2-6E93CBAF5EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2A9F9E-B4C0-41D7-85E8-0273D3543305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,9 +22,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -67,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>FROM:</t>
   </si>
@@ -235,6 +234,9 @@
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -436,7 +438,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -453,6 +455,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -470,15 +473,7 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00;\(0.00\);;\ \ @"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4E4E4"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="21">
     <dxf>
       <font>
         <b/>
@@ -502,108 +497,12 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0;\(0\);;\ \ @"/>
+      <numFmt numFmtId="165" formatCode="0;\(0\);;\ \ @"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFE4E4E4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00;\(0.00\);;\ \ @"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4E4E4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -837,27 +736,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="26"/>
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="totalRow" dxfId="24"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="23"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="22"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="21"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="20"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="19"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="18"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="17"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="16"/>
-      <tableStyleElement type="pageFieldValues" dxfId="15"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="17"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="16"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="15"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="14"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="13"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="12"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="11"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="10"/>
+      <tableStyleElement type="pageFieldValues" dxfId="9"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstColumn" dxfId="11"/>
-      <tableStyleElement type="lastColumn" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="8"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="totalRow" dxfId="6"/>
+      <tableStyleElement type="firstColumn" dxfId="5"/>
+      <tableStyleElement type="lastColumn" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1342,7 +1241,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1677,10 +1576,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B4:L25"/>
+  <dimension ref="B1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1694,6 +1593,11 @@
     <col min="10" max="10" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I1" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
         <v>54</v>
@@ -2126,11 +2030,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I7:L31">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$J7&lt;&gt;""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$I7="Grand Total"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>$J7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -2138,10 +2042,13 @@
       <formula1>_xlfn.ANCHORARRAY($G$6)</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="I1" r:id="rId1" xr:uid="{2528E58B-8B79-452A-B65C-A4F8095F2014}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>